<commit_message>
Correcting some grammar errors
</commit_message>
<xml_diff>
--- a/Sort.xlsx
+++ b/Sort.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>i</t>
   </si>
@@ -21,29 +21,35 @@
     <t>Array</t>
   </si>
   <si>
-    <t>Minimum</t>
+    <t xml:space="preserve">Is there bigger elements?</t>
   </si>
   <si>
-    <t xml:space="preserve">Swap or not</t>
+    <t xml:space="preserve">Insert or not</t>
   </si>
   <si>
-    <t>swap</t>
+    <t>NO</t>
   </si>
   <si>
-    <t xml:space="preserve">don't swap</t>
+    <t>don't</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1, 2</t>
+  </si>
+  <si>
+    <t>Insert</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve">Array sorted</t>
+    <t xml:space="preserve">Array Sorted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -57,11 +63,6 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -72,20 +73,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="0"/>
+        <bgColor theme="0" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0"/>
         <bgColor theme="4" tint="0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="0"/>
-        <bgColor theme="0" tint="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0"/>
-        <bgColor theme="7" tint="0"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor theme="7" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
   </fills>
@@ -153,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,20 +174,20 @@
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="2" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="2" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -699,8 +700,8 @@
   <cols>
     <col min="1" max="1" style="1" width="9.140625"/>
     <col min="2" max="9" width="9.140625"/>
-    <col bestFit="1" min="10" max="10" style="1" width="9.28125"/>
-    <col bestFit="1" min="11" max="11" width="11.421875"/>
+    <col bestFit="1" min="10" max="10" style="1" width="22.421875"/>
+    <col bestFit="1" min="11" max="11" width="11.57421875"/>
     <col min="12" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
@@ -741,23 +742,23 @@
       <c r="E4" s="8">
         <v>2</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>-5</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>0</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <v>32</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>999</v>
       </c>
-      <c r="J4" s="10">
-        <v>-5</v>
-      </c>
-      <c r="K4" s="11" t="s">
+      <c r="J4" s="9" t="s">
         <v>4</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -765,29 +766,29 @@
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2</v>
+      </c>
+      <c r="F5" s="8">
         <v>-5</v>
       </c>
-      <c r="E5" s="13">
-        <v>2</v>
-      </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>0</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <v>32</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>999</v>
       </c>
-      <c r="J5" s="10">
-        <v>0</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>4</v>
+      <c r="J5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" ht="14.25">
@@ -795,29 +796,29 @@
       <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="7">
         <v>-5</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
+        <v>2</v>
+      </c>
+      <c r="G6" s="8">
         <v>0</v>
       </c>
-      <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8">
-        <v>2</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>32</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>999</v>
       </c>
-      <c r="J6" s="10">
-        <v>1</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>5</v>
+      <c r="J6" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" ht="14.25">
@@ -825,13 +826,13 @@
       <c r="C7" s="2">
         <v>3</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="7">
         <v>-5</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="7">
         <v>0</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>1</v>
       </c>
       <c r="G7" s="7">
@@ -840,13 +841,13 @@
       <c r="H7" s="8">
         <v>32</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
         <v>999</v>
       </c>
-      <c r="J7" s="15">
-        <v>2</v>
-      </c>
-      <c r="K7" s="11" t="s">
+      <c r="J7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K7" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -855,59 +856,59 @@
       <c r="C8" s="2">
         <v>4</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="7">
         <v>-5</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="7">
         <v>0</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="7">
         <v>1</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="7">
         <v>2</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="7">
         <v>32</v>
       </c>
       <c r="I8" s="8">
         <v>999</v>
       </c>
-      <c r="J8" s="15">
-        <v>32</v>
-      </c>
-      <c r="K8" s="11" t="s">
+      <c r="J8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="14">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7">
         <v>-5</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="7">
         <v>0</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="7">
         <v>1</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>2</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <v>32</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="7">
         <v>999</v>
       </c>
-      <c r="J9" s="18" t="s">
-        <v>6</v>
+      <c r="J9" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" ht="14.25">

</xml_diff>

<commit_message>
Adding the desription of Merge Sort
</commit_message>
<xml_diff>
--- a/Sort.xlsx
+++ b/Sort.xlsx
@@ -13,46 +13,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>i</t>
+    <t xml:space="preserve">Initial Array</t>
   </si>
   <si>
-    <t>Array</t>
+    <t xml:space="preserve">Get middle</t>
   </si>
   <si>
-    <t xml:space="preserve">Is there bigger elements?</t>
+    <t>Divide</t>
   </si>
   <si>
-    <t xml:space="preserve">Insert or not</t>
+    <t xml:space="preserve">Base Case return</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>don't</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1, 2</t>
-  </si>
-  <si>
-    <t>Insert</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Array Sorted</t>
+    <t>Merge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF9C6500"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -64,12 +55,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -85,12 +82,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor theme="9" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor theme="7" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -99,18 +108,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -150,53 +162,755 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="2" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="4" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="8" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="5" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="11" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="6" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="7" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="13" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="14" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="16" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf fontId="0" fillId="3" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="17" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>314323</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="314324" y="1533524"/>
+          <a:ext cx="342899" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedRightArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 25000"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+            <a:gd name="adj3" fmla="val 25000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>268604</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>27357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>371473</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>170233</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="2268854" y="1656133"/>
+          <a:ext cx="102870" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>369569</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="3543299" y="1266824"/>
+          <a:ext cx="102870" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>8572</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>62098</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>151447</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>164968</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="2851920" flipH="0" flipV="0">
+          <a:off x="1362074" y="1670870"/>
+          <a:ext cx="102870" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590548</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="914399" y="1123949"/>
+          <a:ext cx="342898" cy="1562099"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedRightArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 25000"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+            <a:gd name="adj3" fmla="val 25000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>27357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>93344</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>170233</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="2340314" flipH="0" flipV="0">
+          <a:off x="4486274" y="1656133"/>
+          <a:ext cx="102870" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>27357</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>360044</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>170233</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="5362574" y="1656133"/>
+          <a:ext cx="102870" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>223678</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>566577</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>123823</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="4109878" y="1533524"/>
+          <a:ext cx="342898" cy="942973"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedRightArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 25000"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+            <a:gd name="adj3" fmla="val 25000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>369569</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="6591299" y="1266824"/>
+          <a:ext cx="102870" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 0"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="7086599" y="1171575"/>
+          <a:ext cx="323849" cy="1514474"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedLeftArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 25000"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+            <a:gd name="adj3" fmla="val 25000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="" hidden="0"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="0" flipV="0">
+          <a:off x="6429375" y="752475"/>
+          <a:ext cx="323848" cy="2257424"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedLeftArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 25000"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+            <a:gd name="adj3" fmla="val 25000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
@@ -698,239 +1412,626 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625"/>
-    <col min="2" max="9" width="9.140625"/>
-    <col bestFit="1" min="10" max="10" style="1" width="22.421875"/>
-    <col bestFit="1" min="11" max="11" width="11.57421875"/>
-    <col min="12" max="16384" width="9.140625"/>
+    <col bestFit="1" min="1" max="4" width="10.00390625"/>
+    <col min="5" max="9" width="9.140625"/>
+    <col customWidth="1" min="10" max="11" width="9.140625"/>
+    <col min="12" max="14" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="15" max="15" width="25.140625"/>
+    <col min="16" max="16384" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2">
+        <v>4</v>
+      </c>
+      <c r="J1" s="2">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="8">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8">
+        <v>-5</v>
+      </c>
+      <c r="H3" s="8">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="I3" s="8">
+        <v>32</v>
+      </c>
+      <c r="J3" s="8">
+        <v>999</v>
+      </c>
+      <c r="K3" s="7"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="1"/>
-      <c r="C4" s="2">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>2</v>
+      </c>
+      <c r="G4" s="9">
+        <v>-5</v>
+      </c>
+      <c r="H4" s="8">
         <v>0</v>
       </c>
-      <c r="D4" s="7">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8">
-        <v>2</v>
-      </c>
-      <c r="F4" s="7">
-        <v>-5</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" s="7">
+      <c r="I4" s="8">
         <v>32</v>
       </c>
-      <c r="I4" s="7">
+      <c r="J4" s="8">
         <v>999</v>
       </c>
-      <c r="J4" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="1"/>
-      <c r="C5" s="2">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="11">
+        <v>-5</v>
+      </c>
+      <c r="F5" s="11">
         <v>1</v>
       </c>
-      <c r="D5" s="11">
-        <v>1</v>
-      </c>
-      <c r="E5" s="11">
+      <c r="G5" s="11">
         <v>2</v>
       </c>
-      <c r="F5" s="8">
-        <v>-5</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="H5" s="11">
         <v>0</v>
       </c>
-      <c r="H5" s="7">
+      <c r="I5" s="11">
         <v>32</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="11">
         <v>999</v>
       </c>
-      <c r="J5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>7</v>
-      </c>
+      <c r="K5" s="12"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="1"/>
-      <c r="C6" s="2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="9">
         <v>2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="F6" s="8">
         <v>-5</v>
       </c>
-      <c r="E6" s="12">
-        <v>1</v>
-      </c>
-      <c r="F6" s="12">
-        <v>2</v>
-      </c>
-      <c r="G6" s="8">
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="8">
         <v>0</v>
       </c>
-      <c r="H6" s="7">
+      <c r="J6" s="9">
         <v>32</v>
       </c>
-      <c r="I6" s="7">
+      <c r="K6" s="8">
         <v>999</v>
       </c>
-      <c r="J6" s="13">
-        <v>1.2</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>7</v>
-      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="1"/>
-      <c r="C7" s="2">
-        <v>3</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="B7" s="1"/>
+      <c r="C7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11">
+        <v>2</v>
+      </c>
+      <c r="F7" s="15">
         <v>-5</v>
       </c>
-      <c r="E7" s="7">
+      <c r="G7" s="7"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11">
         <v>0</v>
       </c>
-      <c r="F7" s="7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7">
-        <v>2</v>
-      </c>
-      <c r="H7" s="8">
+      <c r="J7" s="11">
         <v>32</v>
       </c>
-      <c r="I7" s="7">
+      <c r="K7" s="15">
         <v>999</v>
       </c>
-      <c r="J7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="L7" s="7"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="1"/>
-      <c r="C8" s="2">
-        <v>4</v>
-      </c>
-      <c r="D8" s="7">
-        <v>-5</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="9">
         <v>0</v>
       </c>
-      <c r="F8" s="7">
-        <v>1</v>
-      </c>
-      <c r="G8" s="7">
-        <v>2</v>
-      </c>
-      <c r="H8" s="7">
+      <c r="I8" s="8">
         <v>32</v>
       </c>
-      <c r="I8" s="8">
-        <v>999</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>5</v>
-      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="1"/>
-      <c r="C9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="7">
-        <v>-5</v>
-      </c>
-      <c r="E9" s="7">
+      <c r="B9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="17">
+        <v>1</v>
+      </c>
+      <c r="D9" s="15">
+        <v>2</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="17">
         <v>0</v>
       </c>
-      <c r="F9" s="7">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7">
-        <v>2</v>
-      </c>
-      <c r="H9" s="7">
+      <c r="I9" s="15">
         <v>32</v>
       </c>
-      <c r="I9" s="7">
-        <v>999</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="1"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" ht="14.25">
-      <c r="J11" s="1"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" ht="28.5">
+      <c r="A11" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="22">
+        <v>1</v>
+      </c>
+      <c r="D11" s="23">
+        <v>2</v>
+      </c>
+      <c r="E11" s="24"/>
+      <c r="F11" s="23">
+        <v>-5</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="23">
+        <v>0</v>
+      </c>
+      <c r="I11" s="23">
+        <v>32</v>
+      </c>
+      <c r="J11" s="24"/>
+      <c r="K11" s="23">
+        <v>999</v>
+      </c>
+      <c r="L11" s="7"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
     </row>
     <row r="12" ht="14.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
       <c r="J12" s="1"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="J13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="11">
+        <v>1</v>
+      </c>
+      <c r="D13" s="11">
+        <v>2</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <v>32</v>
+      </c>
+      <c r="J13" s="12"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="11">
+        <v>-5</v>
+      </c>
+      <c r="D14" s="11">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="11">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11">
+        <v>32</v>
+      </c>
+      <c r="J14" s="11">
+        <v>999</v>
+      </c>
+      <c r="K14" s="7"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="11">
+        <v>-5</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
+      <c r="H16" s="11">
+        <v>2</v>
+      </c>
+      <c r="I16" s="11">
+        <v>32</v>
+      </c>
+      <c r="J16" s="11">
+        <v>999</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D3:I3"/>
+    <mergeCell ref="E2:J2"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
   <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>